<commit_message>
Final Results in Excel
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philliphuang/Repos/cs124-mst/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philliphuang\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,8 +24,43 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>t0</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>t3</t>
+  </si>
+  <si>
+    <t>t4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimesion 0 </t>
+  </si>
+  <si>
+    <t>Dimension 2</t>
+  </si>
+  <si>
+    <t>Dimension 3</t>
+  </si>
+  <si>
+    <t>Dimension 4</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -57,8 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -68,6 +104,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -336,77 +375,599 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>128</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2.067574</v>
+      </c>
+      <c r="C2" s="1">
+        <v>9.2079740000000001</v>
+      </c>
+      <c r="D2" s="2">
+        <v>20.259508</v>
+      </c>
+      <c r="E2" s="2">
+        <v>29.486353000000001</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2.4399999999999999E-4</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.75E-4</v>
+      </c>
+      <c r="I2">
+        <v>1.2799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2*2</f>
+        <v>256</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2.2171470000000002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>13.48085</v>
+      </c>
+      <c r="D3" s="2">
+        <v>32.268841000000002</v>
+      </c>
+      <c r="E3" s="2">
+        <v>50.056773999999997</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5.7399999999999997E-4</v>
+      </c>
+      <c r="G3" s="2">
+        <v>5.5599999999999996E-4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>4.26E-4</v>
+      </c>
+      <c r="I3">
+        <v>2.52E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3*2</f>
+        <v>512</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.2819029999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <v>19.255382999999998</v>
+      </c>
+      <c r="D4" s="2">
+        <v>50.322609</v>
+      </c>
+      <c r="E4" s="2">
+        <v>83.728485000000006</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.6739999999999999E-3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2.5850000000000001E-3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.5690000000000001E-3</v>
+      </c>
+      <c r="I4">
+        <v>7.3800000000000005E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>A4*2</f>
+        <v>1024</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2.2823799999999999</v>
+      </c>
+      <c r="C5" s="1">
+        <v>26.700358999999999</v>
+      </c>
+      <c r="D5" s="2">
+        <v>80.417297000000005</v>
+      </c>
+      <c r="E5" s="2">
+        <v>137.46104399999999</v>
+      </c>
+      <c r="F5" s="2">
+        <v>6.7879999999999998E-3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3.3960000000000001E-3</v>
+      </c>
+      <c r="I5">
+        <v>1.3749999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>A5*2</f>
+        <v>2048</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.295976</v>
+      </c>
+      <c r="C6" s="1">
+        <v>38.050303999999997</v>
+      </c>
+      <c r="D6" s="2">
+        <v>126.27815200000001</v>
+      </c>
+      <c r="E6" s="2">
+        <v>826.97497599999997</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.1029000000000001E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.0585000000000001E-2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>8.8559999999999993E-3</v>
+      </c>
+      <c r="I6">
+        <v>2.8579999999999999E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>A6*2</f>
+        <v>4096</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.3093659999999998</v>
+      </c>
+      <c r="C7" s="1">
+        <v>53.540801999999999</v>
+      </c>
+      <c r="D7" s="2">
+        <v>198.21266199999999</v>
+      </c>
+      <c r="E7" s="2">
+        <v>777.26031499999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3.6777999999999998E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3.3426999999999998E-2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2.7289999999999998E-2</v>
+      </c>
+      <c r="I7">
+        <v>6.1510000000000002E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>A7*2</f>
+        <v>8192</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2.3254869999999999</v>
+      </c>
+      <c r="C8" s="1">
+        <v>75.186522999999994</v>
+      </c>
+      <c r="D8" s="2">
+        <v>313.823395</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3422.5046390000002</v>
+      </c>
+      <c r="F8" s="2">
+        <v>9.2351000000000003E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>9.0762999999999996E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>7.8902E-2</v>
+      </c>
+      <c r="I8">
+        <v>1.2638999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>A8*2</f>
+        <v>16384</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2.306305</v>
+      </c>
+      <c r="C9" s="1">
+        <v>107.696884</v>
+      </c>
+      <c r="D9" s="2">
+        <v>495.74920700000001</v>
+      </c>
+      <c r="E9" s="2">
+        <v>14021.731444999999</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.18747900000000001</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.23633499999999999</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.201242</v>
+      </c>
+      <c r="I9">
+        <v>3.1465E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>A9*2</f>
+        <v>32768</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2.362374</v>
+      </c>
+      <c r="C10" s="1">
+        <v>150.802582</v>
+      </c>
+      <c r="D10" s="2">
+        <v>779.55127000000005</v>
+      </c>
+      <c r="E10" s="2">
+        <v>47668.335937999997</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.45315100000000003</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.52588299999999999</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.47328300000000001</v>
+      </c>
+      <c r="I10">
+        <v>6.8579000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>A10*2</f>
+        <v>65536</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2.3401679999999998</v>
+      </c>
+      <c r="C11" s="1">
+        <v>212.95133999999999</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1235.3618160000001</v>
+      </c>
+      <c r="E11" s="2">
+        <v>143702.75</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.94422300000000003</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.181028</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.0438229999999999</v>
+      </c>
+      <c r="I11">
+        <v>0.14980299999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>A11*2</f>
+        <v>131072</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.357494</v>
+      </c>
+      <c r="C12" s="1">
+        <v>301.31509399999999</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1956.062866</v>
+      </c>
+      <c r="E12" s="2">
+        <v>579103.5625</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2.0395310000000002</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2.6210040000000001</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2.3082630000000002</v>
+      </c>
+      <c r="I12">
+        <v>0.30135299999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1">
+    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>128</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <f>A1*2</f>
+      <c r="B3" s="2">
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.4399999999999999E-4</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.75E-4</v>
+      </c>
+      <c r="E3">
+        <v>1.2799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3*2</f>
         <v>256</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <f t="shared" ref="A3:A12" si="0">A2*2</f>
+      <c r="B4" s="2">
+        <v>5.7399999999999997E-4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5.5599999999999996E-4</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4.26E-4</v>
+      </c>
+      <c r="E4">
+        <v>2.52E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>A4*2</f>
         <v>512</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <f t="shared" si="0"/>
+      <c r="B5" s="2">
+        <v>1.6739999999999999E-3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2.5850000000000001E-3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.5690000000000001E-3</v>
+      </c>
+      <c r="E5">
+        <v>7.3800000000000005E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>A5*2</f>
         <v>1024</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <f t="shared" si="0"/>
+      <c r="B6" s="2">
+        <v>6.7879999999999998E-3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.3960000000000001E-3</v>
+      </c>
+      <c r="E6">
+        <v>1.3749999999999999E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>A6*2</f>
         <v>2048</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <f t="shared" si="0"/>
+      <c r="B7" s="2">
+        <v>1.1029000000000001E-2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.0585000000000001E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>8.8559999999999993E-3</v>
+      </c>
+      <c r="E7">
+        <v>2.8579999999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>A7*2</f>
         <v>4096</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <f t="shared" si="0"/>
+      <c r="B8" s="2">
+        <v>3.6777999999999998E-2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3.3426999999999998E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.7289999999999998E-2</v>
+      </c>
+      <c r="E8">
+        <v>6.1510000000000002E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>A8*2</f>
         <v>8192</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>16384</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>32768</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
+        <v>9.2351000000000003E-2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>9.0762999999999996E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7.8902E-2</v>
+      </c>
+      <c r="E9">
+        <v>1.2638999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A9*2</f>
+        <v>16384</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.18747900000000001</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.23633499999999999</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.201242</v>
+      </c>
+      <c r="E10">
+        <v>3.1465E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>A10*2</f>
+        <v>32768</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.45315100000000003</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.52588299999999999</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.47328300000000001</v>
+      </c>
+      <c r="E11">
+        <v>6.8579000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>A11*2</f>
         <v>65536</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <f t="shared" si="0"/>
+      <c r="B12" s="2">
+        <v>0.94422300000000003</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.181028</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.0438229999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.14980299999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>A12*2</f>
         <v>131072</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2.0395310000000002</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2.6210040000000001</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2.3082630000000002</v>
+      </c>
+      <c r="E13">
+        <v>0.30135299999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>